<commit_message>
trying to run ATPU model with LESP code, so far unsuccessful...
</commit_message>
<xml_diff>
--- a/data/ATPU_trend_data_SEGupdate.xlsx
+++ b/data/ATPU_trend_data_SEGupdate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GutowskyS\Documents\Petrel_Puffin_Trend\Petrel_Puffin_Trend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DF3F0ECD-C9A7-4E08-B6A8-D4DB14CC6360}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3E1FF0B-7765-4F40-A3C6-599FDE2619A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="46">
   <si>
     <t>Country</t>
   </si>
@@ -159,6 +159,21 @@
   </si>
   <si>
     <t>NorthShore MB Sanctuaries , QC</t>
+  </si>
+  <si>
+    <t>Machias Seal Island, NB</t>
+  </si>
+  <si>
+    <t>Baccalieu Island, NF</t>
+  </si>
+  <si>
+    <t>North Bird Island, NF</t>
+  </si>
+  <si>
+    <t>Puffin Islands (Lab), LB</t>
+  </si>
+  <si>
+    <t>S. Wilhelm, ?</t>
   </si>
 </sst>
 </file>
@@ -497,11 +512,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K78"/>
+  <dimension ref="A1:K103"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D67" sqref="D67"/>
+      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I109" sqref="I109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2366,23 +2381,611 @@
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="D74" s="1"/>
+      <c r="A74" t="s">
+        <v>11</v>
+      </c>
+      <c r="B74" t="s">
+        <v>41</v>
+      </c>
+      <c r="C74">
+        <v>1965</v>
+      </c>
+      <c r="D74">
+        <v>3000</v>
+      </c>
       <c r="H74" s="1"/>
+      <c r="J74" t="s">
+        <v>45</v>
+      </c>
+      <c r="K74" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="D75" s="1"/>
+      <c r="A75" t="s">
+        <v>11</v>
+      </c>
+      <c r="B75" t="s">
+        <v>41</v>
+      </c>
+      <c r="C75">
+        <v>1971</v>
+      </c>
+      <c r="D75">
+        <v>3000</v>
+      </c>
       <c r="H75" s="1"/>
+      <c r="J75" t="s">
+        <v>45</v>
+      </c>
+      <c r="K75" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A76" t="s">
+        <v>11</v>
+      </c>
+      <c r="B76" t="s">
+        <v>41</v>
+      </c>
+      <c r="C76">
+        <v>1974</v>
+      </c>
+      <c r="D76">
+        <v>1780</v>
+      </c>
       <c r="H76" s="1"/>
+      <c r="J76" t="s">
+        <v>45</v>
+      </c>
+      <c r="K76" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A77" t="s">
+        <v>11</v>
+      </c>
+      <c r="B77" t="s">
+        <v>41</v>
+      </c>
+      <c r="C77">
+        <v>1975</v>
+      </c>
+      <c r="D77">
+        <v>1500</v>
+      </c>
       <c r="H77" s="1"/>
       <c r="I77" s="1"/>
+      <c r="J77" t="s">
+        <v>45</v>
+      </c>
+      <c r="K77" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A78" t="s">
+        <v>11</v>
+      </c>
+      <c r="B78" t="s">
+        <v>41</v>
+      </c>
+      <c r="C78">
+        <v>1976</v>
+      </c>
+      <c r="D78">
+        <v>4600</v>
+      </c>
       <c r="H78" s="1"/>
       <c r="I78" s="1"/>
+      <c r="J78" t="s">
+        <v>45</v>
+      </c>
+      <c r="K78" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A79" t="s">
+        <v>11</v>
+      </c>
+      <c r="B79" t="s">
+        <v>41</v>
+      </c>
+      <c r="C79">
+        <v>1977</v>
+      </c>
+      <c r="D79">
+        <v>1200</v>
+      </c>
+      <c r="J79" t="s">
+        <v>45</v>
+      </c>
+      <c r="K79" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A80" t="s">
+        <v>11</v>
+      </c>
+      <c r="B80" t="s">
+        <v>41</v>
+      </c>
+      <c r="C80">
+        <v>1978</v>
+      </c>
+      <c r="D80">
+        <v>1100</v>
+      </c>
+      <c r="J80" t="s">
+        <v>45</v>
+      </c>
+      <c r="K80" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A81" t="s">
+        <v>11</v>
+      </c>
+      <c r="B81" t="s">
+        <v>41</v>
+      </c>
+      <c r="C81">
+        <v>1978</v>
+      </c>
+      <c r="D81">
+        <v>3000</v>
+      </c>
+      <c r="J81" t="s">
+        <v>45</v>
+      </c>
+      <c r="K81" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A82" t="s">
+        <v>11</v>
+      </c>
+      <c r="B82" t="s">
+        <v>41</v>
+      </c>
+      <c r="C82">
+        <v>1979</v>
+      </c>
+      <c r="D82">
+        <v>1300</v>
+      </c>
+      <c r="J82" t="s">
+        <v>45</v>
+      </c>
+      <c r="K82" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A83" t="s">
+        <v>11</v>
+      </c>
+      <c r="B83" t="s">
+        <v>41</v>
+      </c>
+      <c r="C83">
+        <v>1979</v>
+      </c>
+      <c r="D83">
+        <v>1626</v>
+      </c>
+      <c r="J83" t="s">
+        <v>45</v>
+      </c>
+      <c r="K83" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A84" t="s">
+        <v>11</v>
+      </c>
+      <c r="B84" t="s">
+        <v>41</v>
+      </c>
+      <c r="C84">
+        <v>1980</v>
+      </c>
+      <c r="D84">
+        <v>1500</v>
+      </c>
+      <c r="J84" t="s">
+        <v>45</v>
+      </c>
+      <c r="K84" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A85" t="s">
+        <v>11</v>
+      </c>
+      <c r="B85" t="s">
+        <v>41</v>
+      </c>
+      <c r="C85">
+        <v>1981</v>
+      </c>
+      <c r="D85">
+        <v>1600</v>
+      </c>
+      <c r="J85" t="s">
+        <v>45</v>
+      </c>
+      <c r="K85" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A86" t="s">
+        <v>11</v>
+      </c>
+      <c r="B86" t="s">
+        <v>41</v>
+      </c>
+      <c r="C86">
+        <v>1982</v>
+      </c>
+      <c r="D86">
+        <v>1600</v>
+      </c>
+      <c r="J86" t="s">
+        <v>45</v>
+      </c>
+      <c r="K86" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A87" t="s">
+        <v>11</v>
+      </c>
+      <c r="B87" t="s">
+        <v>41</v>
+      </c>
+      <c r="C87">
+        <v>1983</v>
+      </c>
+      <c r="D87">
+        <v>1500</v>
+      </c>
+      <c r="J87" t="s">
+        <v>45</v>
+      </c>
+      <c r="K87" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A88" t="s">
+        <v>11</v>
+      </c>
+      <c r="B88" t="s">
+        <v>41</v>
+      </c>
+      <c r="C88">
+        <v>1987</v>
+      </c>
+      <c r="D88">
+        <v>1700</v>
+      </c>
+      <c r="J88" t="s">
+        <v>45</v>
+      </c>
+      <c r="K88" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A89" t="s">
+        <v>11</v>
+      </c>
+      <c r="B89" t="s">
+        <v>41</v>
+      </c>
+      <c r="C89">
+        <v>1998</v>
+      </c>
+      <c r="D89">
+        <v>2000</v>
+      </c>
+      <c r="J89" t="s">
+        <v>45</v>
+      </c>
+      <c r="K89" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A90" t="s">
+        <v>11</v>
+      </c>
+      <c r="B90" t="s">
+        <v>41</v>
+      </c>
+      <c r="C90">
+        <v>2000</v>
+      </c>
+      <c r="D90">
+        <v>16048</v>
+      </c>
+      <c r="J90" t="s">
+        <v>45</v>
+      </c>
+      <c r="K90" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A91" t="s">
+        <v>11</v>
+      </c>
+      <c r="B91" t="s">
+        <v>41</v>
+      </c>
+      <c r="C91">
+        <v>2003</v>
+      </c>
+      <c r="D91">
+        <v>14668</v>
+      </c>
+      <c r="J91" t="s">
+        <v>45</v>
+      </c>
+      <c r="K91" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A92" t="s">
+        <v>11</v>
+      </c>
+      <c r="B92" t="s">
+        <v>41</v>
+      </c>
+      <c r="C92">
+        <v>2011</v>
+      </c>
+      <c r="D92">
+        <v>15676</v>
+      </c>
+      <c r="J92" t="s">
+        <v>45</v>
+      </c>
+      <c r="K92" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A93" t="s">
+        <v>11</v>
+      </c>
+      <c r="B93" t="s">
+        <v>41</v>
+      </c>
+      <c r="C93">
+        <v>2015</v>
+      </c>
+      <c r="D93">
+        <v>10350</v>
+      </c>
+      <c r="J93" t="s">
+        <v>45</v>
+      </c>
+      <c r="K93" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A94" t="s">
+        <v>11</v>
+      </c>
+      <c r="B94" t="s">
+        <v>41</v>
+      </c>
+      <c r="C94">
+        <v>2016</v>
+      </c>
+      <c r="D94">
+        <v>9592</v>
+      </c>
+      <c r="J94" t="s">
+        <v>45</v>
+      </c>
+      <c r="K94" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A95" t="s">
+        <v>11</v>
+      </c>
+      <c r="B95" t="s">
+        <v>41</v>
+      </c>
+      <c r="C95">
+        <v>2019</v>
+      </c>
+      <c r="D95">
+        <v>17270</v>
+      </c>
+      <c r="J95" t="s">
+        <v>45</v>
+      </c>
+      <c r="K95" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A96" t="s">
+        <v>11</v>
+      </c>
+      <c r="B96" t="s">
+        <v>42</v>
+      </c>
+      <c r="C96">
+        <v>1979</v>
+      </c>
+      <c r="D96">
+        <v>58748</v>
+      </c>
+      <c r="J96" t="s">
+        <v>45</v>
+      </c>
+      <c r="K96" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A97" t="s">
+        <v>11</v>
+      </c>
+      <c r="B97" t="s">
+        <v>42</v>
+      </c>
+      <c r="C97">
+        <v>1984</v>
+      </c>
+      <c r="D97">
+        <v>60000</v>
+      </c>
+      <c r="J97" t="s">
+        <v>45</v>
+      </c>
+      <c r="K97" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A98" t="s">
+        <v>11</v>
+      </c>
+      <c r="B98" t="s">
+        <v>42</v>
+      </c>
+      <c r="C98">
+        <v>1996</v>
+      </c>
+      <c r="D98">
+        <v>90600</v>
+      </c>
+      <c r="J98" t="s">
+        <v>45</v>
+      </c>
+      <c r="K98" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A99" t="s">
+        <v>11</v>
+      </c>
+      <c r="B99" t="s">
+        <v>42</v>
+      </c>
+      <c r="C99">
+        <v>2005</v>
+      </c>
+      <c r="D99">
+        <v>150000</v>
+      </c>
+      <c r="J99" t="s">
+        <v>45</v>
+      </c>
+      <c r="K99" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A100" t="s">
+        <v>11</v>
+      </c>
+      <c r="B100" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C100" s="4">
+        <v>1985</v>
+      </c>
+      <c r="D100" s="4">
+        <v>2000</v>
+      </c>
+      <c r="J100" t="s">
+        <v>45</v>
+      </c>
+      <c r="K100" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A101" t="s">
+        <v>11</v>
+      </c>
+      <c r="B101" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C101" s="4">
+        <v>2019</v>
+      </c>
+      <c r="D101" s="4">
+        <v>18782</v>
+      </c>
+      <c r="J101" t="s">
+        <v>45</v>
+      </c>
+      <c r="K101" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A102" t="s">
+        <v>11</v>
+      </c>
+      <c r="B102" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C102" s="4">
+        <v>1978</v>
+      </c>
+      <c r="D102">
+        <v>3894</v>
+      </c>
+      <c r="J102" t="s">
+        <v>45</v>
+      </c>
+      <c r="K102" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A103" t="s">
+        <v>11</v>
+      </c>
+      <c r="B103" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C103" s="4">
+        <v>2002</v>
+      </c>
+      <c r="D103">
+        <v>1238</v>
+      </c>
+      <c r="J103" t="s">
+        <v>45</v>
+      </c>
+      <c r="K103" t="s">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K78">

</xml_diff>

<commit_message>
typo fixed in ATPU data for Great Island 1984 lower CI
</commit_message>
<xml_diff>
--- a/data/ATPU_trend_data_SEGupdate.xlsx
+++ b/data/ATPU_trend_data_SEGupdate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GutowskyS\Documents\Petrel_Puffin_Trend\Petrel_Puffin_Trend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3E1FF0B-7765-4F40-A3C6-599FDE2619A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E58FD8C-1A53-482A-952E-C9FE2FC082CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -515,8 +515,8 @@
   <dimension ref="A1:K103"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I109" sqref="I109"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1689,8 +1689,8 @@
       </c>
       <c r="E44" s="1"/>
       <c r="H44" s="1">
-        <f>159427*2</f>
-        <v>318854</v>
+        <f>129877*2</f>
+        <v>259754</v>
       </c>
       <c r="I44" s="1">
         <f>188977*2</f>

</xml_diff>

<commit_message>
Greg and Sarah got the GAMM fired up and working for ATPU!
</commit_message>
<xml_diff>
--- a/data/ATPU_trend_data_SEGupdate.xlsx
+++ b/data/ATPU_trend_data_SEGupdate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GutowskyS\Documents\Petrel_Puffin_Trend\Petrel_Puffin_Trend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E58FD8C-1A53-482A-952E-C9FE2FC082CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{806B1CA8-AE9A-45F5-8C60-FA636180D294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -203,12 +203,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -223,7 +229,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -232,6 +238,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -515,8 +522,8 @@
   <dimension ref="A1:K103"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F41" sqref="F41"/>
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F85" sqref="F85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2840,8 +2847,8 @@
       <c r="D96">
         <v>58748</v>
       </c>
-      <c r="J96" t="s">
-        <v>45</v>
+      <c r="J96" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="K96" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
updated LESP data to include Country and Little White Island in NS, also MSI but removed because of no SEs and small number but obvious impact on regional trend uncertainty; playing with plotting options, fixing colony-level trajectory plots for facets to be ordered by latitude rather than alphabetical; added some prelim maps of just colonies with counts used for trends
</commit_message>
<xml_diff>
--- a/data/ATPU_trend_data_SEGupdate.xlsx
+++ b/data/ATPU_trend_data_SEGupdate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GutowskyS\Documents\Petrel_Puffin_Trend\Petrel_Puffin_Trend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{806B1CA8-AE9A-45F5-8C60-FA636180D294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E587AE1-A6DC-49BB-AEB0-AFFC22F50EE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26055" yWindow="1935" windowWidth="24075" windowHeight="14265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -74,51 +74,18 @@
     <t>Canada</t>
   </si>
   <si>
-    <t>Bacalhao, LAB</t>
-  </si>
-  <si>
     <t>Robertson et al. 2002</t>
   </si>
   <si>
     <t>S. Wilhelm, unpubl. Data</t>
   </si>
   <si>
-    <t>Tinker, LAB</t>
-  </si>
-  <si>
-    <t>Herring Island 1, LAB</t>
-  </si>
-  <si>
     <t>R. Elliot, unpubl. Report</t>
   </si>
   <si>
-    <t>Herring Island 2, LAB</t>
-  </si>
-  <si>
-    <t>Herring Island 3, LAB</t>
-  </si>
-  <si>
-    <t>North Green, LAB</t>
-  </si>
-  <si>
-    <t>Gannet Clusters 2, LAB</t>
-  </si>
-  <si>
-    <t>Gannet Clusters 3, LAB</t>
-  </si>
-  <si>
-    <t>Gannet Clusters 4, LAB</t>
-  </si>
-  <si>
-    <t>Gannet Clusters 5, LAB</t>
-  </si>
-  <si>
     <t>No SE or other variance provided</t>
   </si>
   <si>
-    <t>Gannet Clusters 6, LAB</t>
-  </si>
-  <si>
     <t>Wilhelm et al. 2015</t>
   </si>
   <si>
@@ -140,40 +107,73 @@
     <t>Jean-François Rail</t>
   </si>
   <si>
-    <t>Pee Pee Island, Witless Bay, NF</t>
-  </si>
-  <si>
-    <t>Great Island, Witless Bay, NF</t>
-  </si>
-  <si>
-    <t>Gull Island, Witless Bay,NF</t>
-  </si>
-  <si>
-    <t>Coleman Island, Wadham Islands,NF</t>
-  </si>
-  <si>
-    <t>South Penguin Island, Wadham Islands, NF</t>
-  </si>
-  <si>
-    <t>Small Island, Wadham Islands, NF</t>
-  </si>
-  <si>
     <t>NorthShore MB Sanctuaries , QC</t>
   </si>
   <si>
     <t>Machias Seal Island, NB</t>
   </si>
   <si>
-    <t>Baccalieu Island, NF</t>
-  </si>
-  <si>
-    <t>North Bird Island, NF</t>
-  </si>
-  <si>
-    <t>Puffin Islands (Lab), LB</t>
-  </si>
-  <si>
     <t>S. Wilhelm, ?</t>
+  </si>
+  <si>
+    <t>Bacalhao, NL</t>
+  </si>
+  <si>
+    <t>Tinker, NL</t>
+  </si>
+  <si>
+    <t>Herring Island 1, NL</t>
+  </si>
+  <si>
+    <t>Herring Island 2, NL</t>
+  </si>
+  <si>
+    <t>Herring Island 3, NL</t>
+  </si>
+  <si>
+    <t>North Green, NL</t>
+  </si>
+  <si>
+    <t>Gannet Clusters 2, NL</t>
+  </si>
+  <si>
+    <t>Gannet Clusters 3, NL</t>
+  </si>
+  <si>
+    <t>Gannet Clusters 4, NL</t>
+  </si>
+  <si>
+    <t>Gannet Clusters 5, NL</t>
+  </si>
+  <si>
+    <t>Gannet Clusters 6, NL</t>
+  </si>
+  <si>
+    <t>Baccalieu Island, NL</t>
+  </si>
+  <si>
+    <t>North Bird Island, NL</t>
+  </si>
+  <si>
+    <t>Pee Pee Island, NL</t>
+  </si>
+  <si>
+    <t>Great Island, NL</t>
+  </si>
+  <si>
+    <t>Gull Island, NL</t>
+  </si>
+  <si>
+    <t>Coleman Island, NL</t>
+  </si>
+  <si>
+    <t>South Penguin Island, NL</t>
+  </si>
+  <si>
+    <t>Small Island, NL</t>
+  </si>
+  <si>
+    <t>Puffin Islands, NL</t>
   </si>
 </sst>
 </file>
@@ -522,8 +522,8 @@
   <dimension ref="A1:K103"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F85" sqref="F85"/>
+      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B87" sqref="B87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -574,7 +574,7 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="C2">
         <v>1978</v>
@@ -594,7 +594,7 @@
         <v>166</v>
       </c>
       <c r="J2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -602,7 +602,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="C3">
         <v>2002</v>
@@ -621,7 +621,7 @@
         <v>130</v>
       </c>
       <c r="J3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -629,7 +629,7 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="C4">
         <v>2010</v>
@@ -648,7 +648,7 @@
         <v>88</v>
       </c>
       <c r="J4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -656,7 +656,7 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="C5">
         <v>1978</v>
@@ -675,7 +675,7 @@
         <v>80</v>
       </c>
       <c r="J5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -683,7 +683,7 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="C6">
         <v>2002</v>
@@ -703,7 +703,7 @@
         <v>72</v>
       </c>
       <c r="J6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -711,7 +711,7 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="C7">
         <v>2010</v>
@@ -730,7 +730,7 @@
         <v>18</v>
       </c>
       <c r="J7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -738,7 +738,7 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C8">
         <v>1978</v>
@@ -761,7 +761,7 @@
         <v>9814</v>
       </c>
       <c r="J8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -769,7 +769,7 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C9">
         <v>2010</v>
@@ -792,7 +792,7 @@
         <v>4910</v>
       </c>
       <c r="J9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -800,7 +800,7 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="C10">
         <v>1978</v>
@@ -823,7 +823,7 @@
         <v>18652</v>
       </c>
       <c r="J10" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -831,7 +831,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="C11">
         <v>2010</v>
@@ -854,7 +854,7 @@
         <v>19952</v>
       </c>
       <c r="J11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -862,7 +862,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="C12">
         <v>1978</v>
@@ -883,7 +883,7 @@
         <v>9218</v>
       </c>
       <c r="J12" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -891,7 +891,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="C13">
         <v>2010</v>
@@ -913,7 +913,7 @@
         <v>5520</v>
       </c>
       <c r="J13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -921,7 +921,7 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="C14">
         <v>1978</v>
@@ -944,7 +944,7 @@
         <v>6652</v>
       </c>
       <c r="J14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -952,7 +952,7 @@
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="C15" s="4">
         <v>2002</v>
@@ -975,7 +975,7 @@
         <v>7120</v>
       </c>
       <c r="J15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -983,7 +983,7 @@
         <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="C16">
         <v>2010</v>
@@ -1006,7 +1006,7 @@
         <v>9710</v>
       </c>
       <c r="J16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1014,7 +1014,7 @@
         <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="C17">
         <v>1978</v>
@@ -1031,7 +1031,7 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1039,7 +1039,7 @@
         <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="C18">
         <v>1983</v>
@@ -1055,7 +1055,7 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1063,7 +1063,7 @@
         <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="C19">
         <v>1984</v>
@@ -1080,7 +1080,7 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1088,7 +1088,7 @@
         <v>11</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="C20">
         <v>1999</v>
@@ -1105,7 +1105,7 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1113,7 +1113,7 @@
         <v>11</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="C21">
         <v>2015</v>
@@ -1130,7 +1130,7 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1138,7 +1138,7 @@
         <v>11</v>
       </c>
       <c r="B22" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="C22">
         <v>1978</v>
@@ -1155,7 +1155,7 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1163,7 +1163,7 @@
         <v>11</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="C23">
         <v>1983</v>
@@ -1179,7 +1179,7 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1187,7 +1187,7 @@
         <v>11</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="C24">
         <v>1984</v>
@@ -1204,7 +1204,7 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1212,7 +1212,7 @@
         <v>11</v>
       </c>
       <c r="B25" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="C25">
         <v>1999</v>
@@ -1229,7 +1229,7 @@
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1237,7 +1237,7 @@
         <v>11</v>
       </c>
       <c r="B26" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="C26">
         <v>2018</v>
@@ -1254,7 +1254,7 @@
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1262,7 +1262,7 @@
         <v>11</v>
       </c>
       <c r="B27" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="C27">
         <v>1978</v>
@@ -1279,7 +1279,7 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1287,7 +1287,7 @@
         <v>11</v>
       </c>
       <c r="B28" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="C28">
         <v>1983</v>
@@ -1303,7 +1303,7 @@
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1311,7 +1311,7 @@
         <v>11</v>
       </c>
       <c r="B29" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="C29">
         <v>1984</v>
@@ -1328,7 +1328,7 @@
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1336,7 +1336,7 @@
         <v>11</v>
       </c>
       <c r="B30" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="C30">
         <v>1999</v>
@@ -1353,7 +1353,7 @@
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1361,7 +1361,7 @@
         <v>11</v>
       </c>
       <c r="B31" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="C31">
         <v>2015</v>
@@ -1378,7 +1378,7 @@
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1386,7 +1386,7 @@
         <v>11</v>
       </c>
       <c r="B32" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="C32">
         <v>1978</v>
@@ -1400,10 +1400,10 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="K32" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1411,7 +1411,7 @@
         <v>11</v>
       </c>
       <c r="B33" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="C33">
         <v>1983</v>
@@ -1428,7 +1428,7 @@
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1436,7 +1436,7 @@
         <v>11</v>
       </c>
       <c r="B34" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="C34">
         <v>1984</v>
@@ -1453,7 +1453,7 @@
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
       <c r="J34" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1461,7 +1461,7 @@
         <v>11</v>
       </c>
       <c r="B35" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="C35">
         <v>1999</v>
@@ -1477,7 +1477,7 @@
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
       <c r="J35" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1485,7 +1485,7 @@
         <v>11</v>
       </c>
       <c r="B36" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="C36">
         <v>2018</v>
@@ -1502,7 +1502,7 @@
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
       <c r="J36" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1510,7 +1510,7 @@
         <v>11</v>
       </c>
       <c r="B37" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="C37">
         <v>1983</v>
@@ -1527,7 +1527,7 @@
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
       <c r="J37" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1535,7 +1535,7 @@
         <v>11</v>
       </c>
       <c r="B38" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="C38" s="4">
         <v>1984</v>
@@ -1551,7 +1551,7 @@
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
       <c r="J38" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1559,7 +1559,7 @@
         <v>11</v>
       </c>
       <c r="B39" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="C39" s="4">
         <v>1999</v>
@@ -1575,7 +1575,7 @@
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
       <c r="J39" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1583,7 +1583,7 @@
         <v>11</v>
       </c>
       <c r="B40" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="C40">
         <v>2018</v>
@@ -1599,7 +1599,7 @@
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
       <c r="J40" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1607,7 +1607,7 @@
         <v>11</v>
       </c>
       <c r="B41" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C41">
         <v>1979</v>
@@ -1624,7 +1624,7 @@
         <v>5000</v>
       </c>
       <c r="J41" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1632,7 +1632,7 @@
         <v>11</v>
       </c>
       <c r="B42" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C42">
         <v>2010</v>
@@ -1649,7 +1649,7 @@
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
       <c r="J42" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1657,7 +1657,7 @@
         <v>11</v>
       </c>
       <c r="B43" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C43">
         <v>1979</v>
@@ -1677,7 +1677,7 @@
         <v>252224</v>
       </c>
       <c r="J43" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1685,7 +1685,7 @@
         <v>11</v>
       </c>
       <c r="B44" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C44">
         <v>1984</v>
@@ -1704,7 +1704,7 @@
         <v>377954</v>
       </c>
       <c r="J44" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1712,7 +1712,7 @@
         <v>11</v>
       </c>
       <c r="B45" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C45">
         <v>1985</v>
@@ -1731,7 +1731,7 @@
         <v>349834</v>
       </c>
       <c r="J45" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1739,7 +1739,7 @@
         <v>11</v>
       </c>
       <c r="B46" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C46">
         <v>1993</v>
@@ -1759,7 +1759,7 @@
         <v>461040</v>
       </c>
       <c r="J46" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1767,7 +1767,7 @@
         <v>11</v>
       </c>
       <c r="B47" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C47">
         <v>2011</v>
@@ -1787,7 +1787,7 @@
         <v>402846</v>
       </c>
       <c r="J47" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1795,7 +1795,7 @@
         <v>11</v>
       </c>
       <c r="B48" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C48">
         <v>1979</v>
@@ -1813,7 +1813,7 @@
         <v>90000</v>
       </c>
       <c r="J48" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1821,7 +1821,7 @@
         <v>11</v>
       </c>
       <c r="B49" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C49">
         <v>1984</v>
@@ -1837,7 +1837,7 @@
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
       <c r="J49" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1845,7 +1845,7 @@
         <v>11</v>
       </c>
       <c r="B50" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C50">
         <v>1985</v>
@@ -1861,7 +1861,7 @@
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
       <c r="J50" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1869,7 +1869,7 @@
         <v>11</v>
       </c>
       <c r="B51" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C51">
         <v>2003</v>
@@ -1886,7 +1886,7 @@
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
       <c r="J51" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1894,7 +1894,7 @@
         <v>11</v>
       </c>
       <c r="B52" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C52">
         <v>2012</v>
@@ -1909,7 +1909,7 @@
       </c>
       <c r="H52" s="1"/>
       <c r="J52" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1917,7 +1917,7 @@
         <v>11</v>
       </c>
       <c r="B53" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C53">
         <v>2023</v>
@@ -1932,7 +1932,7 @@
       </c>
       <c r="H53" s="1"/>
       <c r="J53" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1940,7 +1940,7 @@
         <v>11</v>
       </c>
       <c r="B54" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C54" s="4">
         <v>1979</v>
@@ -1958,7 +1958,7 @@
         <v>978</v>
       </c>
       <c r="J54" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1966,7 +1966,7 @@
         <v>11</v>
       </c>
       <c r="B55" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C55" s="4">
         <v>2018</v>
@@ -1981,7 +1981,7 @@
       </c>
       <c r="H55" s="1"/>
       <c r="J55" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1989,7 +1989,7 @@
         <v>11</v>
       </c>
       <c r="B56" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C56" s="4">
         <v>1979</v>
@@ -2001,7 +2001,7 @@
       <c r="E56" s="1"/>
       <c r="H56" s="1"/>
       <c r="J56" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2009,7 +2009,7 @@
         <v>11</v>
       </c>
       <c r="B57" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C57" s="4">
         <v>2018</v>
@@ -2024,7 +2024,7 @@
       </c>
       <c r="H57" s="1"/>
       <c r="J57" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2032,7 +2032,7 @@
         <v>11</v>
       </c>
       <c r="B58" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C58" s="4">
         <v>1979</v>
@@ -2051,7 +2051,7 @@
         <v>54844.800000000003</v>
       </c>
       <c r="J58" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2059,7 +2059,7 @@
         <v>11</v>
       </c>
       <c r="B59" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C59" s="4">
         <v>1980</v>
@@ -2075,7 +2075,7 @@
       <c r="H59" s="1"/>
       <c r="I59" s="1"/>
       <c r="J59" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2083,7 +2083,7 @@
         <v>11</v>
       </c>
       <c r="B60" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C60" s="4">
         <v>1984</v>
@@ -2099,7 +2099,7 @@
       <c r="H60" s="1"/>
       <c r="I60" s="1"/>
       <c r="J60" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2107,7 +2107,7 @@
         <v>11</v>
       </c>
       <c r="B61" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C61" s="4">
         <v>2001</v>
@@ -2123,7 +2123,7 @@
       <c r="H61" s="1"/>
       <c r="I61" s="1"/>
       <c r="J61" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2131,7 +2131,7 @@
         <v>11</v>
       </c>
       <c r="B62" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C62" s="4">
         <v>2018</v>
@@ -2147,7 +2147,7 @@
       <c r="H62" s="1"/>
       <c r="I62" s="1"/>
       <c r="J62" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2155,7 +2155,7 @@
         <v>11</v>
       </c>
       <c r="B63" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="C63">
         <v>1965</v>
@@ -2167,10 +2167,10 @@
       <c r="H63" s="1"/>
       <c r="I63" s="1"/>
       <c r="J63" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="K63" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2178,7 +2178,7 @@
         <v>11</v>
       </c>
       <c r="B64" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="C64">
         <v>1972</v>
@@ -2190,10 +2190,10 @@
       <c r="H64" s="1"/>
       <c r="I64" s="1"/>
       <c r="J64" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="K64" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2201,7 +2201,7 @@
         <v>11</v>
       </c>
       <c r="B65" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="C65">
         <v>1977</v>
@@ -2212,10 +2212,10 @@
       <c r="E65" s="1"/>
       <c r="H65" s="1"/>
       <c r="J65" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="K65" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2223,7 +2223,7 @@
         <v>11</v>
       </c>
       <c r="B66" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="C66">
         <v>1982</v>
@@ -2234,10 +2234,10 @@
       <c r="E66" s="1"/>
       <c r="H66" s="1"/>
       <c r="J66" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="K66" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2245,7 +2245,7 @@
         <v>11</v>
       </c>
       <c r="B67" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="C67">
         <v>1988</v>
@@ -2255,10 +2255,10 @@
       </c>
       <c r="H67" s="1"/>
       <c r="J67" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="K67" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2266,7 +2266,7 @@
         <v>11</v>
       </c>
       <c r="B68" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="C68">
         <v>1993</v>
@@ -2276,10 +2276,10 @@
       </c>
       <c r="H68" s="1"/>
       <c r="J68" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="K68" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2287,7 +2287,7 @@
         <v>11</v>
       </c>
       <c r="B69" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="C69">
         <v>1998</v>
@@ -2297,10 +2297,10 @@
       </c>
       <c r="H69" s="1"/>
       <c r="J69" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="K69" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2308,7 +2308,7 @@
         <v>11</v>
       </c>
       <c r="B70" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="C70">
         <v>2005</v>
@@ -2318,10 +2318,10 @@
       </c>
       <c r="H70" s="1"/>
       <c r="J70" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="K70" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2329,7 +2329,7 @@
         <v>11</v>
       </c>
       <c r="B71" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="C71">
         <v>2010</v>
@@ -2339,10 +2339,10 @@
       </c>
       <c r="H71" s="1"/>
       <c r="J71" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="K71" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2350,7 +2350,7 @@
         <v>11</v>
       </c>
       <c r="B72" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="C72">
         <v>2015</v>
@@ -2360,10 +2360,10 @@
       </c>
       <c r="H72" s="1"/>
       <c r="J72" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="K72" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2371,7 +2371,7 @@
         <v>11</v>
       </c>
       <c r="B73" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="C73">
         <v>2022</v>
@@ -2381,10 +2381,10 @@
       </c>
       <c r="H73" s="1"/>
       <c r="J73" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="K73" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2392,7 +2392,7 @@
         <v>11</v>
       </c>
       <c r="B74" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="C74">
         <v>1965</v>
@@ -2402,10 +2402,10 @@
       </c>
       <c r="H74" s="1"/>
       <c r="J74" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="K74" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2413,7 +2413,7 @@
         <v>11</v>
       </c>
       <c r="B75" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="C75">
         <v>1971</v>
@@ -2423,10 +2423,10 @@
       </c>
       <c r="H75" s="1"/>
       <c r="J75" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="K75" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2434,7 +2434,7 @@
         <v>11</v>
       </c>
       <c r="B76" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="C76">
         <v>1974</v>
@@ -2444,10 +2444,10 @@
       </c>
       <c r="H76" s="1"/>
       <c r="J76" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="K76" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2455,7 +2455,7 @@
         <v>11</v>
       </c>
       <c r="B77" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="C77">
         <v>1975</v>
@@ -2466,10 +2466,10 @@
       <c r="H77" s="1"/>
       <c r="I77" s="1"/>
       <c r="J77" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="K77" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2477,7 +2477,7 @@
         <v>11</v>
       </c>
       <c r="B78" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="C78">
         <v>1976</v>
@@ -2488,10 +2488,10 @@
       <c r="H78" s="1"/>
       <c r="I78" s="1"/>
       <c r="J78" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="K78" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2499,7 +2499,7 @@
         <v>11</v>
       </c>
       <c r="B79" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="C79">
         <v>1977</v>
@@ -2508,10 +2508,10 @@
         <v>1200</v>
       </c>
       <c r="J79" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="K79" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2519,7 +2519,7 @@
         <v>11</v>
       </c>
       <c r="B80" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="C80">
         <v>1978</v>
@@ -2528,10 +2528,10 @@
         <v>1100</v>
       </c>
       <c r="J80" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="K80" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2539,7 +2539,7 @@
         <v>11</v>
       </c>
       <c r="B81" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="C81">
         <v>1978</v>
@@ -2548,10 +2548,10 @@
         <v>3000</v>
       </c>
       <c r="J81" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="K81" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2559,7 +2559,7 @@
         <v>11</v>
       </c>
       <c r="B82" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="C82">
         <v>1979</v>
@@ -2568,10 +2568,10 @@
         <v>1300</v>
       </c>
       <c r="J82" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="K82" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2579,7 +2579,7 @@
         <v>11</v>
       </c>
       <c r="B83" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="C83">
         <v>1979</v>
@@ -2588,10 +2588,10 @@
         <v>1626</v>
       </c>
       <c r="J83" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="K83" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2599,7 +2599,7 @@
         <v>11</v>
       </c>
       <c r="B84" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="C84">
         <v>1980</v>
@@ -2608,10 +2608,10 @@
         <v>1500</v>
       </c>
       <c r="J84" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="K84" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2619,7 +2619,7 @@
         <v>11</v>
       </c>
       <c r="B85" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="C85">
         <v>1981</v>
@@ -2628,10 +2628,10 @@
         <v>1600</v>
       </c>
       <c r="J85" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="K85" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2639,7 +2639,7 @@
         <v>11</v>
       </c>
       <c r="B86" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="C86">
         <v>1982</v>
@@ -2648,10 +2648,10 @@
         <v>1600</v>
       </c>
       <c r="J86" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="K86" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2659,7 +2659,7 @@
         <v>11</v>
       </c>
       <c r="B87" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="C87">
         <v>1983</v>
@@ -2668,10 +2668,10 @@
         <v>1500</v>
       </c>
       <c r="J87" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="K87" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2679,7 +2679,7 @@
         <v>11</v>
       </c>
       <c r="B88" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="C88">
         <v>1987</v>
@@ -2688,10 +2688,10 @@
         <v>1700</v>
       </c>
       <c r="J88" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="K88" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2699,7 +2699,7 @@
         <v>11</v>
       </c>
       <c r="B89" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="C89">
         <v>1998</v>
@@ -2708,10 +2708,10 @@
         <v>2000</v>
       </c>
       <c r="J89" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="K89" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2719,7 +2719,7 @@
         <v>11</v>
       </c>
       <c r="B90" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="C90">
         <v>2000</v>
@@ -2728,10 +2728,10 @@
         <v>16048</v>
       </c>
       <c r="J90" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="K90" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2739,7 +2739,7 @@
         <v>11</v>
       </c>
       <c r="B91" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="C91">
         <v>2003</v>
@@ -2748,10 +2748,10 @@
         <v>14668</v>
       </c>
       <c r="J91" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="K91" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2759,7 +2759,7 @@
         <v>11</v>
       </c>
       <c r="B92" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="C92">
         <v>2011</v>
@@ -2768,10 +2768,10 @@
         <v>15676</v>
       </c>
       <c r="J92" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="K92" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2779,7 +2779,7 @@
         <v>11</v>
       </c>
       <c r="B93" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="C93">
         <v>2015</v>
@@ -2788,10 +2788,10 @@
         <v>10350</v>
       </c>
       <c r="J93" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="K93" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2799,7 +2799,7 @@
         <v>11</v>
       </c>
       <c r="B94" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="C94">
         <v>2016</v>
@@ -2808,10 +2808,10 @@
         <v>9592</v>
       </c>
       <c r="J94" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="K94" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2819,7 +2819,7 @@
         <v>11</v>
       </c>
       <c r="B95" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="C95">
         <v>2019</v>
@@ -2828,10 +2828,10 @@
         <v>17270</v>
       </c>
       <c r="J95" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="K95" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2839,7 +2839,7 @@
         <v>11</v>
       </c>
       <c r="B96" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C96">
         <v>1979</v>
@@ -2848,10 +2848,10 @@
         <v>58748</v>
       </c>
       <c r="J96" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K96" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2859,7 +2859,7 @@
         <v>11</v>
       </c>
       <c r="B97" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C97">
         <v>1984</v>
@@ -2868,10 +2868,10 @@
         <v>60000</v>
       </c>
       <c r="J97" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="K97" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2879,7 +2879,7 @@
         <v>11</v>
       </c>
       <c r="B98" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C98">
         <v>1996</v>
@@ -2888,10 +2888,10 @@
         <v>90600</v>
       </c>
       <c r="J98" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="K98" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2899,7 +2899,7 @@
         <v>11</v>
       </c>
       <c r="B99" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C99">
         <v>2005</v>
@@ -2908,10 +2908,10 @@
         <v>150000</v>
       </c>
       <c r="J99" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="K99" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2919,7 +2919,7 @@
         <v>11</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C100" s="4">
         <v>1985</v>
@@ -2928,10 +2928,10 @@
         <v>2000</v>
       </c>
       <c r="J100" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="K100" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2939,7 +2939,7 @@
         <v>11</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C101" s="4">
         <v>2019</v>
@@ -2948,10 +2948,10 @@
         <v>18782</v>
       </c>
       <c r="J101" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="K101" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2959,7 +2959,7 @@
         <v>11</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C102" s="4">
         <v>1978</v>
@@ -2968,10 +2968,10 @@
         <v>3894</v>
       </c>
       <c r="J102" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="K102" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2979,7 +2979,7 @@
         <v>11</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C103" s="4">
         <v>2002</v>
@@ -2988,10 +2988,10 @@
         <v>1238</v>
       </c>
       <c r="J103" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="K103" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
re-ran simulation with 15 colonies instead of 9 (took 22 hours to run)
</commit_message>
<xml_diff>
--- a/data/ATPU_trend_data_SEGupdate.xlsx
+++ b/data/ATPU_trend_data_SEGupdate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GutowskyS\Documents\Petrel_Puffin_Trend\Petrel_Puffin_Trend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E587AE1-A6DC-49BB-AEB0-AFFC22F50EE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9011D83-E23E-46E7-8D3B-6023DE4E3160}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26055" yWindow="1935" windowWidth="24075" windowHeight="14265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="180" yWindow="264" windowWidth="21462" windowHeight="13104" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="47">
   <si>
     <t>Country</t>
   </si>
@@ -174,6 +174,9 @@
   </si>
   <si>
     <t>Puffin Islands, NL</t>
+  </si>
+  <si>
+    <t>assuming complete hole count but still no SE</t>
   </si>
 </sst>
 </file>
@@ -522,8 +525,8 @@
   <dimension ref="A1:K103"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B87" sqref="B87"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K93" sqref="K93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2404,9 +2407,6 @@
       <c r="J74" t="s">
         <v>25</v>
       </c>
-      <c r="K74" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" t="s">
@@ -2425,9 +2425,6 @@
       <c r="J75" t="s">
         <v>25</v>
       </c>
-      <c r="K75" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" t="s">
@@ -2445,9 +2442,6 @@
       <c r="H76" s="1"/>
       <c r="J76" t="s">
         <v>25</v>
-      </c>
-      <c r="K76" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2468,9 +2462,6 @@
       <c r="J77" t="s">
         <v>25</v>
       </c>
-      <c r="K77" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" t="s">
@@ -2490,9 +2481,6 @@
       <c r="J78" t="s">
         <v>25</v>
       </c>
-      <c r="K78" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" t="s">
@@ -2510,9 +2498,6 @@
       <c r="J79" t="s">
         <v>25</v>
       </c>
-      <c r="K79" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" t="s">
@@ -2530,9 +2515,6 @@
       <c r="J80" t="s">
         <v>25</v>
       </c>
-      <c r="K80" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" t="s">
@@ -2550,9 +2532,6 @@
       <c r="J81" t="s">
         <v>25</v>
       </c>
-      <c r="K81" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" t="s">
@@ -2570,9 +2549,6 @@
       <c r="J82" t="s">
         <v>25</v>
       </c>
-      <c r="K82" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" t="s">
@@ -2590,9 +2566,6 @@
       <c r="J83" t="s">
         <v>25</v>
       </c>
-      <c r="K83" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" t="s">
@@ -2610,9 +2583,6 @@
       <c r="J84" t="s">
         <v>25</v>
       </c>
-      <c r="K84" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" t="s">
@@ -2630,9 +2600,6 @@
       <c r="J85" t="s">
         <v>25</v>
       </c>
-      <c r="K85" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" t="s">
@@ -2650,9 +2617,6 @@
       <c r="J86" t="s">
         <v>25</v>
       </c>
-      <c r="K86" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" t="s">
@@ -2670,9 +2634,6 @@
       <c r="J87" t="s">
         <v>25</v>
       </c>
-      <c r="K87" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" t="s">
@@ -2690,9 +2651,6 @@
       <c r="J88" t="s">
         <v>25</v>
       </c>
-      <c r="K88" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" t="s">
@@ -2710,9 +2668,6 @@
       <c r="J89" t="s">
         <v>25</v>
       </c>
-      <c r="K89" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" t="s">
@@ -2731,7 +2686,7 @@
         <v>25</v>
       </c>
       <c r="K90" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2751,7 +2706,7 @@
         <v>25</v>
       </c>
       <c r="K91" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2771,7 +2726,7 @@
         <v>25</v>
       </c>
       <c r="K92" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2791,7 +2746,7 @@
         <v>25</v>
       </c>
       <c r="K93" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2811,7 +2766,7 @@
         <v>25</v>
       </c>
       <c r="K94" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2831,7 +2786,7 @@
         <v>25</v>
       </c>
       <c r="K95" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.55000000000000004">

</xml_diff>